<commit_message>
New Version of techmap --> Needs debugging in process
</commit_message>
<xml_diff>
--- a/Data/Techmap/DEModel_V2.xlsx
+++ b/Data/Techmap/DEModel_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT-OTHER\CESM\Data\Techmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255D9439-9A0F-47F1-8739-947D2587B4D2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDC1798-F1AD-41C3-AC21-5E1304AFA082}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10236" yWindow="120" windowWidth="6492" windowHeight="8172" activeTab="4" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
+    <workbookView xWindow="10236" yWindow="120" windowWidth="6492" windowHeight="8172" activeTab="3" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="9" r:id="rId1"/>
@@ -939,8 +939,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{74A02AEB-67CD-4D1C-8FE9-7365E46D98F4}" name="Tabelle4" displayName="Tabelle4" ref="A1:D63" totalsRowShown="0">
-  <autoFilter ref="A1:D63" xr:uid="{A4F2E66D-1024-44EB-B26C-9EF3C2ACFA7D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{74A02AEB-67CD-4D1C-8FE9-7365E46D98F4}" name="Tabelle4" displayName="Tabelle4" ref="A1:D64" totalsRowShown="0">
+  <autoFilter ref="A1:D64" xr:uid="{A4F2E66D-1024-44EB-B26C-9EF3C2ACFA7D}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{68045503-4D44-4DCF-9110-03DFC110F65E}" name="conversion_process_name"/>
     <tableColumn id="2" xr3:uid="{B201BB8F-62F7-4A39-95D4-A92A4057D6C7}" name="description"/>
@@ -1782,10 +1782,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70369A52-6DA6-442B-A9B0-7FE85C1EDFA1}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2214,28 +2214,32 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="58" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="9" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="9" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2252,11 +2256,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042B031A-8F6B-4A01-B2DE-DD19A2E3D336}">
   <dimension ref="A1:Z93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="I29" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N34" sqref="N34"/>
+      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated Model version with important bug fixes. Not 100% validaded.
</commit_message>
<xml_diff>
--- a/Data/Techmap/DEModel_V2.xlsx
+++ b/Data/Techmap/DEModel_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT-OTHER\CESM\Data\Techmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDC1798-F1AD-41C3-AC21-5E1304AFA082}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E79E48-C675-4536-99CB-C05AB44A28A7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10236" yWindow="120" windowWidth="6492" windowHeight="8172" activeTab="3" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
+    <workbookView xWindow="10236" yWindow="120" windowWidth="6492" windowHeight="8172" activeTab="4" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="245">
   <si>
     <t>Base</t>
   </si>
@@ -353,9 +353,6 @@
     <t>Mio EUR</t>
   </si>
   <si>
-    <t>test-tss</t>
-  </si>
-  <si>
     <t>is_storage</t>
   </si>
   <si>
@@ -765,6 +762,15 @@
   </si>
   <si>
     <t>[2016 0;2035 355]</t>
+  </si>
+  <si>
+    <t>[2016 870; 2030 540; 2050 240; 2060 140]</t>
+  </si>
+  <si>
+    <t>test_tss</t>
+  </si>
+  <si>
+    <t>[2016 14.3;2017 NaN]</t>
   </si>
 </sst>
 </file>
@@ -861,7 +867,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -891,6 +897,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1298,7 +1307,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1308,13 +1317,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>123</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1343,7 +1352,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="str">
         <f>IF(B2="kW","t",IF(B2="MW","kilo t","Mio t"))</f>
@@ -1373,8 +1382,7 @@
         <v>35</v>
       </c>
       <c r="C6">
-        <f>IF(Power = "GW", 10^3,IF(Power ="MW",10^3,1))/10^6</f>
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1391,7 +1399,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
         <v>104</v>
@@ -1415,15 +1423,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C314D8A4-C600-4AA7-912A-1904B77A7F29}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.77734375" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" customWidth="1"/>
     <col min="5" max="5" width="15.21875" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
@@ -1432,10 +1440,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
         <v>118</v>
-      </c>
-      <c r="B1" t="s">
-        <v>119</v>
       </c>
       <c r="C1" t="s">
         <v>43</v>
@@ -1444,13 +1452,13 @@
         <v>44</v>
       </c>
       <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" t="s">
         <v>120</v>
-      </c>
-      <c r="F1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" t="s">
-        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>28</v>
@@ -1463,8 +1471,8 @@
       <c r="B2">
         <v>0.05</v>
       </c>
-      <c r="C2" t="s">
-        <v>101</v>
+      <c r="C2" s="15" t="s">
+        <v>242</v>
       </c>
       <c r="E2">
         <v>2015</v>
@@ -1481,7 +1489,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B3">
         <v>0.05</v>
@@ -1496,7 +1504,7 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>105</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1576,7 +1584,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1587,21 +1595,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
         <v>144</v>
-      </c>
-      <c r="D1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1624,7 +1632,7 @@
         <v>88</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D6" s="4">
         <v>10</v>
@@ -1640,7 +1648,7 @@
         <v>86</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D8" s="4">
         <v>10</v>
@@ -1651,7 +1659,7 @@
         <v>84</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D9" s="4">
         <v>10</v>
@@ -1662,7 +1670,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D10" s="4">
         <v>10</v>
@@ -1673,7 +1681,7 @@
         <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D11" s="4">
         <v>10</v>
@@ -1684,7 +1692,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D12" s="4">
         <v>10</v>
@@ -1695,7 +1703,7 @@
         <v>47</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D13" s="4">
         <v>10</v>
@@ -1706,7 +1714,7 @@
         <v>80</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D14" s="4">
         <v>10</v>
@@ -1717,7 +1725,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D15" s="4">
         <v>10</v>
@@ -1728,7 +1736,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D16" s="4">
         <v>10</v>
@@ -1739,7 +1747,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D17" s="4">
         <v>10</v>
@@ -1750,7 +1758,7 @@
         <v>76</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D18" s="4">
         <v>11</v>
@@ -1758,17 +1766,17 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -1784,8 +1792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70369A52-6DA6-442B-A9B0-7FE85C1EDFA1}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1796,16 +1804,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
         <v>144</v>
-      </c>
-      <c r="D1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1813,7 +1821,7 @@
         <v>71</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1824,7 +1832,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -1835,7 +1843,7 @@
         <v>72</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -1846,7 +1854,7 @@
         <v>74</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -1857,7 +1865,7 @@
         <v>75</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" s="4">
         <v>4</v>
@@ -1868,7 +1876,7 @@
         <v>77</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D8" s="4">
         <v>5</v>
@@ -1879,7 +1887,7 @@
         <v>78</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D9" s="4">
         <v>6</v>
@@ -1943,7 +1951,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D19" s="9">
         <v>0</v>
@@ -1956,10 +1964,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D22" s="4">
         <v>10</v>
@@ -1967,29 +1975,29 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -1997,10 +2005,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D29" s="4">
         <v>10</v>
@@ -2008,32 +2016,32 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D36" s="4">
         <v>10</v>
@@ -2042,10 +2050,10 @@
     <row r="37" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D38" s="4">
         <v>9</v>
@@ -2053,10 +2061,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D39" s="4">
         <v>11</v>
@@ -2064,10 +2072,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D40" s="4">
         <v>4</v>
@@ -2076,10 +2084,10 @@
     <row r="41" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D42">
         <v>30</v>
@@ -2087,10 +2095,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D43" s="9">
         <v>31</v>
@@ -2098,10 +2106,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D44" s="9">
         <v>32</v>
@@ -2109,10 +2117,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D45">
         <v>33</v>
@@ -2120,10 +2128,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D46" s="4">
         <v>34</v>
@@ -2131,10 +2139,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D47" s="4">
         <v>35</v>
@@ -2142,7 +2150,7 @@
     </row>
     <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B48"/>
       <c r="C48"/>
@@ -2151,15 +2159,15 @@
     <row r="49" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D51" s="4">
         <v>10</v>
@@ -2167,15 +2175,15 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D53" s="4">
         <v>9</v>
@@ -2183,10 +2191,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D54" s="4">
         <v>3</v>
@@ -2197,7 +2205,7 @@
         <v>50</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D56" s="4">
         <v>10</v>
@@ -2208,7 +2216,7 @@
         <v>49</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D57" s="4">
         <v>10</v>
@@ -2220,27 +2228,27 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2256,19 +2264,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042B031A-8F6B-4A01-B2DE-DD19A2E3D336}">
   <dimension ref="A1:Z93"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="K59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
+      <selection pane="bottomRight" activeCell="N71" sqref="N71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" customWidth="1"/>
     <col min="7" max="9" width="10.77734375" customWidth="1"/>
@@ -2293,25 +2301,25 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" t="s">
         <v>126</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>127</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>128</v>
       </c>
-      <c r="D1" t="s">
-        <v>129</v>
-      </c>
       <c r="E1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="H1" t="s">
         <v>40</v>
@@ -2365,21 +2373,21 @@
         <v>100</v>
       </c>
       <c r="Y1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z1" t="s">
         <v>114</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="7" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>23</v>
@@ -2388,13 +2396,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>99</v>
@@ -2418,16 +2426,16 @@
         <v>68</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X2" s="7" t="s">
         <v>70</v>
       </c>
       <c r="Y2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z2" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2543,7 +2551,7 @@
       <c r="N5" s="6"/>
       <c r="O5" s="5"/>
       <c r="P5" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
@@ -2583,7 +2591,7 @@
       <c r="N6" s="6"/>
       <c r="O6" s="5"/>
       <c r="P6" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
@@ -2663,7 +2671,7 @@
       <c r="N8" s="6"/>
       <c r="O8" s="5"/>
       <c r="P8" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
@@ -2754,13 +2762,13 @@
     </row>
     <row r="11" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>0</v>
@@ -2779,7 +2787,7 @@
       <c r="N11" s="6"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
@@ -2854,13 +2862,13 @@
     </row>
     <row r="14" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>0</v>
@@ -2888,13 +2896,13 @@
     </row>
     <row r="15" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>0</v>
@@ -2970,7 +2978,7 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="T17" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
@@ -3168,7 +3176,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>80</v>
@@ -3229,7 +3237,7 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>45</v>
@@ -3250,11 +3258,11 @@
         <v>0.86</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L25" s="6"/>
       <c r="N25" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O25" s="5">
         <v>30</v>
@@ -3263,7 +3271,7 @@
         <v>165</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S25" s="5"/>
       <c r="T25" s="6"/>
@@ -3276,7 +3284,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>18</v>
@@ -3297,11 +3305,11 @@
         <v>0.86</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L26" s="5"/>
       <c r="N26" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O26" s="5">
         <v>40</v>
@@ -3323,10 +3331,10 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>19</v>
@@ -3344,11 +3352,11 @@
         <v>0.95</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L27" s="5"/>
       <c r="N27" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O27" s="5">
         <v>25</v>
@@ -3370,7 +3378,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>48</v>
@@ -3391,11 +3399,11 @@
         <v>0.76</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L28" s="5"/>
       <c r="N28" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O28" s="5">
         <v>40</v>
@@ -3417,7 +3425,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>47</v>
@@ -3438,11 +3446,11 @@
         <v>0.95</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L29" s="5"/>
       <c r="N29" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O29" s="5">
         <v>60</v>
@@ -3491,7 +3499,7 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>17</v>
@@ -3510,11 +3518,11 @@
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L31" s="6"/>
       <c r="N31" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O31" s="5"/>
       <c r="Q31" s="6">
@@ -3534,7 +3542,7 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>17</v>
@@ -3557,7 +3565,7 @@
       </c>
       <c r="L32" s="6"/>
       <c r="N32" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O32" s="5">
         <v>25</v>
@@ -3566,7 +3574,7 @@
         <v>15</v>
       </c>
       <c r="R32" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S32" s="5"/>
       <c r="T32" s="6"/>
@@ -3581,7 +3589,7 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>17</v>
@@ -3626,7 +3634,7 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>17</v>
@@ -3645,13 +3653,13 @@
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O34" s="5"/>
       <c r="Q34" s="6">
@@ -3671,7 +3679,7 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>17</v>
@@ -3694,7 +3702,7 @@
       </c>
       <c r="L35" s="6"/>
       <c r="N35" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O35" s="5">
         <v>25</v>
@@ -3703,7 +3711,7 @@
         <v>93</v>
       </c>
       <c r="R35" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S35" s="5"/>
       <c r="T35" s="6"/>
@@ -3718,7 +3726,7 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>17</v>
@@ -3737,13 +3745,13 @@
       </c>
       <c r="J36" s="6"/>
       <c r="K36" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O36" s="5"/>
       <c r="Q36" s="6">
@@ -3763,7 +3771,7 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>17</v>
@@ -3786,7 +3794,7 @@
       </c>
       <c r="L37" s="6"/>
       <c r="N37" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O37" s="5">
         <v>25</v>
@@ -3795,7 +3803,7 @@
         <v>13</v>
       </c>
       <c r="R37" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="S37" s="5"/>
       <c r="T37" s="6"/>
@@ -3810,7 +3818,7 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>18</v>
@@ -3854,7 +3862,7 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>19</v>
@@ -3898,10 +3906,10 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>84</v>
@@ -3938,7 +3946,7 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>84</v>
@@ -3970,7 +3978,7 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>45</v>
@@ -4010,7 +4018,7 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>19</v>
@@ -4037,7 +4045,7 @@
         <v>1.5</v>
       </c>
       <c r="R47" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S47" s="5"/>
       <c r="T47" s="6"/>
@@ -4050,7 +4058,7 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>46</v>
@@ -4135,13 +4143,13 @@
       </c>
       <c r="J50" s="6"/>
       <c r="K50" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="N50" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="L50" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="N50" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="O50" s="5">
         <v>25</v>
@@ -4150,15 +4158,15 @@
         <v>1.93</v>
       </c>
       <c r="R50" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S50" s="5"/>
       <c r="T50" s="6"/>
       <c r="U50" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="V50" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
@@ -4192,7 +4200,7 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>45</v>
@@ -4211,10 +4219,10 @@
       </c>
       <c r="J52" s="6"/>
       <c r="K52" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N52" s="5" t="s">
         <v>93</v>
@@ -4226,12 +4234,12 @@
         <v>20</v>
       </c>
       <c r="R52" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="S52" s="5"/>
       <c r="T52" s="6"/>
       <c r="U52" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
@@ -4243,10 +4251,10 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>82</v>
@@ -4262,10 +4270,10 @@
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N53" s="5" t="s">
         <v>94</v>
@@ -4277,12 +4285,12 @@
         <v>10</v>
       </c>
       <c r="R53" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="S53" s="5"/>
       <c r="T53" s="6"/>
       <c r="U53" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V53" s="3">
         <v>0.55000000000000004</v>
@@ -4296,7 +4304,7 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>19</v>
@@ -4326,12 +4334,12 @@
         <v>18</v>
       </c>
       <c r="R54" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S54" s="5"/>
       <c r="T54" s="6"/>
       <c r="U54" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="V54" s="3"/>
       <c r="W54" s="3"/>
@@ -4343,7 +4351,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>80</v>
@@ -4362,10 +4370,10 @@
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N55" s="5" t="s">
         <v>95</v>
@@ -4377,12 +4385,12 @@
         <v>15</v>
       </c>
       <c r="R55" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S55" s="5"/>
       <c r="T55" s="6"/>
       <c r="U55" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="V55" s="3"/>
       <c r="W55" s="3"/>
@@ -4394,7 +4402,7 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>19</v>
@@ -4424,12 +4432,12 @@
         <v>15</v>
       </c>
       <c r="R56" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S56" s="5"/>
       <c r="T56" s="6"/>
       <c r="U56" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
@@ -4489,7 +4497,7 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>45</v>
@@ -4523,7 +4531,7 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>91</v>
@@ -4559,7 +4567,7 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>91</v>
@@ -4609,7 +4617,7 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>91</v>
@@ -4667,7 +4675,7 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>18</v>
@@ -4701,7 +4709,7 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>92</v>
@@ -4735,7 +4743,7 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>92</v>
@@ -4754,10 +4762,10 @@
         <v>0.75</v>
       </c>
       <c r="K66" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="L66" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="L66" s="5" t="s">
-        <v>181</v>
       </c>
       <c r="N66" s="6"/>
       <c r="O66" s="5">
@@ -4785,7 +4793,7 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>92</v>
@@ -4843,13 +4851,13 @@
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>0</v>
@@ -4879,10 +4887,10 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>17</v>
@@ -4913,10 +4921,10 @@
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>19</v>
@@ -4930,11 +4938,11 @@
       <c r="I71" s="3"/>
       <c r="J71" s="6"/>
       <c r="K71" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L71" s="5"/>
-      <c r="N71" s="5" t="s">
-        <v>179</v>
+      <c r="N71" s="6" t="s">
+        <v>244</v>
       </c>
       <c r="O71" s="5">
         <v>30</v>
@@ -4960,10 +4968,10 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>86</v>
@@ -4992,10 +5000,10 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="K73" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.3">
@@ -5073,7 +5081,7 @@
         <v>450</v>
       </c>
       <c r="R75" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S75" s="4"/>
       <c r="T75" s="4"/>
@@ -5088,13 +5096,13 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B76" t="s">
         <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D76" t="s">
         <v>0</v>
@@ -5103,10 +5111,10 @@
         <v>0.7</v>
       </c>
       <c r="Q76" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R76" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S76">
         <v>0</v>
@@ -5119,13 +5127,13 @@
     </row>
     <row r="78" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B78" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>0</v>
@@ -5139,10 +5147,10 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>88</v>
@@ -5153,10 +5161,10 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>82</v>
@@ -5167,10 +5175,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>86</v>
@@ -5181,10 +5189,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>84</v>
@@ -5195,10 +5203,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>19</v>
@@ -5209,10 +5217,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C84" s="9" t="s">
         <v>45</v>
@@ -5223,10 +5231,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C85" s="9" t="s">
         <v>46</v>
@@ -5237,10 +5245,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>47</v>
@@ -5251,10 +5259,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C87" s="9" t="s">
         <v>80</v>
@@ -5265,10 +5273,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C88" s="9" t="s">
         <v>73</v>
@@ -5279,10 +5287,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C89" s="9" t="s">
         <v>48</v>
@@ -5293,10 +5301,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C90" s="9" t="s">
         <v>18</v>
@@ -5307,10 +5315,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C91" s="9" t="s">
         <v>76</v>
@@ -5321,13 +5329,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>0</v>
@@ -5335,13 +5343,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D93" s="9" t="s">
         <v>0</v>
@@ -5361,7 +5369,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5394,7 +5402,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>243</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
empty line is allowed in commodities tab
</commit_message>
<xml_diff>
--- a/Data/Techmap/DEModel_V2.xlsx
+++ b/Data/Techmap/DEModel_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sina Hajikazemi\Documents\mycode\CESM\Data\Techmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384775DC-BD00-4082-8D9D-E8863518ACCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A05E5A-DC16-47F4-97C8-D64EF3AB2460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11175" activeTab="4" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{EC78BDD3-7137-425A-8228-7CE92A9A1C25}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="9" r:id="rId1"/>
@@ -941,8 +941,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C14D454B-12DF-41D4-B756-57EA49F00895}" name="Tabelle3" displayName="Tabelle3" ref="A1:D21" totalsRowShown="0">
-  <autoFilter ref="A1:D21" xr:uid="{801D801C-681D-47E7-ACE2-316227FD6501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C14D454B-12DF-41D4-B756-57EA49F00895}" name="Tabelle3" displayName="Tabelle3" ref="A1:D22" totalsRowShown="0">
+  <autoFilter ref="A1:D22" xr:uid="{801D801C-681D-47E7-ACE2-316227FD6501}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0AF4638F-3EEB-48E0-AC29-8DF8557BEA8D}" name="commodity_name"/>
     <tableColumn id="2" xr3:uid="{C6986DB7-7572-49F8-AEB6-52667D90A759}" name="description"/>
@@ -1316,12 +1316,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>120</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -1433,18 +1433,18 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="36.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>116</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>238</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -1587,19 +1587,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0387EA4-7159-4CF0-ABE0-71D3891C6DB9}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -1613,122 +1613,112 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D7" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="D8" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="D9" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>161</v>
+        <v>83</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>158</v>
       </c>
       <c r="D10" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>150</v>
+        <v>45</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="D12" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>149</v>
+        <v>46</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>150</v>
       </c>
       <c r="D13" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>146</v>
+        <v>47</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="D14" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>146</v>
@@ -1737,51 +1727,62 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>147</v>
+        <v>72</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="D16" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>145</v>
+        <v>48</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="D17" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D19" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>235</v>
       </c>
     </row>
@@ -1799,16 +1800,16 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -1822,7 +1823,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1833,7 +1834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -1877,7 +1878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1899,7 +1900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>78</v>
       </c>
@@ -1907,7 +1908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>80</v>
       </c>
@@ -1915,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1923,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -1931,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -1939,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -1955,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>164</v>
       </c>
@@ -1963,12 +1964,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>221</v>
       </c>
@@ -1979,29 +1980,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>223</v>
       </c>
       <c r="C25" s="9"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>212</v>
       </c>
@@ -2009,7 +2010,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>211</v>
       </c>
@@ -2020,29 +2021,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>210</v>
       </c>
@@ -2053,8 +2054,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>166</v>
       </c>
@@ -2065,7 +2066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -2076,7 +2077,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>167</v>
       </c>
@@ -2087,8 +2088,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>195</v>
       </c>
@@ -2099,7 +2100,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>196</v>
       </c>
@@ -2110,7 +2111,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>197</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>198</v>
       </c>
@@ -2132,7 +2133,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>199</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>200</v>
       </c>
@@ -2154,7 +2155,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>173</v>
       </c>
@@ -2162,13 +2163,13 @@
       <c r="C48"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>169</v>
       </c>
@@ -2179,12 +2180,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>171</v>
       </c>
@@ -2195,7 +2196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>172</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>50</v>
       </c>
@@ -2217,7 +2218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -2228,31 +2229,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>235</v>
       </c>
@@ -2270,42 +2271,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042B031A-8F6B-4A01-B2DE-DD19A2E3D336}">
   <dimension ref="A1:Z93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K74" sqref="K74:L74"/>
+      <selection pane="bottomRight" activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
-    <col min="11" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="7" max="9" width="10.7265625" customWidth="1"/>
+    <col min="10" max="10" width="20.26953125" customWidth="1"/>
+    <col min="11" max="12" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7265625" customWidth="1"/>
+    <col min="14" max="14" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7265625" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17.7265625" customWidth="1"/>
     <col min="18" max="18" width="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="13.28515625" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" customWidth="1"/>
-    <col min="24" max="24" width="13.7109375" customWidth="1"/>
-    <col min="25" max="25" width="17.28515625" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" customWidth="1"/>
+    <col min="19" max="19" width="15.7265625" customWidth="1"/>
+    <col min="20" max="20" width="13.26953125" customWidth="1"/>
+    <col min="21" max="21" width="14.26953125" customWidth="1"/>
+    <col min="22" max="22" width="14.453125" customWidth="1"/>
+    <col min="23" max="23" width="12.7265625" customWidth="1"/>
+    <col min="24" max="24" width="13.7265625" customWidth="1"/>
+    <col min="25" max="25" width="17.26953125" customWidth="1"/>
+    <col min="26" max="26" width="16.26953125" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -2385,7 +2386,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="7" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="7" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E2" s="11" t="s">
         <v>106</v>
       </c>
@@ -2444,7 +2445,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -2488,7 +2489,7 @@
         <v>TWh/a</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>70</v>
       </c>
@@ -2530,7 +2531,7 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -2570,7 +2571,7 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>71</v>
       </c>
@@ -2610,7 +2611,7 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>73</v>
       </c>
@@ -2650,7 +2651,7 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>74</v>
       </c>
@@ -2690,7 +2691,7 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>76</v>
       </c>
@@ -2727,7 +2728,7 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>77</v>
       </c>
@@ -2766,7 +2767,7 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>133</v>
       </c>
@@ -2808,7 +2809,7 @@
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2832,7 +2833,7 @@
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>78</v>
       </c>
@@ -2866,7 +2867,7 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
     </row>
-    <row r="14" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>136</v>
       </c>
@@ -2900,7 +2901,7 @@
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
     </row>
-    <row r="15" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>137</v>
       </c>
@@ -2934,7 +2935,7 @@
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2958,7 +2959,7 @@
       <c r="Y16" s="6"/>
       <c r="Z16" s="6"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>80</v>
       </c>
@@ -2995,7 +2996,7 @@
       </c>
       <c r="Z17" s="6"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -3032,7 +3033,7 @@
       </c>
       <c r="Z18" s="6"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>82</v>
       </c>
@@ -3069,7 +3070,7 @@
       </c>
       <c r="Z19" s="6"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>84</v>
       </c>
@@ -3106,7 +3107,7 @@
       </c>
       <c r="Z20" s="6"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>86</v>
       </c>
@@ -3143,7 +3144,7 @@
       </c>
       <c r="Z21" s="6"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>88</v>
       </c>
@@ -3180,7 +3181,7 @@
       </c>
       <c r="Z22" s="6"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>164</v>
       </c>
@@ -3217,7 +3218,7 @@
       </c>
       <c r="Z23" s="6"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -3241,7 +3242,7 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>172</v>
       </c>
@@ -3288,7 +3289,7 @@
       <c r="Y25" s="6"/>
       <c r="Z25" s="6"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>171</v>
       </c>
@@ -3335,7 +3336,7 @@
       <c r="Y26" s="6"/>
       <c r="Z26" s="6"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>170</v>
       </c>
@@ -3382,7 +3383,7 @@
       <c r="Y27" s="6"/>
       <c r="Z27" s="6"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>169</v>
       </c>
@@ -3429,7 +3430,7 @@
       <c r="Y28" s="6"/>
       <c r="Z28" s="6"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>168</v>
       </c>
@@ -3478,7 +3479,7 @@
       </c>
       <c r="Z29" s="6"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -3503,7 +3504,7 @@
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>199</v>
       </c>
@@ -3546,7 +3547,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>200</v>
       </c>
@@ -3593,7 +3594,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>173</v>
       </c>
@@ -3638,7 +3639,7 @@
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>195</v>
       </c>
@@ -3683,7 +3684,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>196</v>
       </c>
@@ -3730,7 +3731,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>197</v>
       </c>
@@ -3775,7 +3776,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>198</v>
       </c>
@@ -3822,7 +3823,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>210</v>
       </c>
@@ -3866,7 +3867,7 @@
       <c r="Y40" s="6"/>
       <c r="Z40" s="6"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>209</v>
       </c>
@@ -3910,7 +3911,7 @@
       </c>
       <c r="Z41" s="6"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>208</v>
       </c>
@@ -3950,7 +3951,7 @@
       <c r="Y42" s="6"/>
       <c r="Z42" s="6"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>174</v>
       </c>
@@ -3982,7 +3983,7 @@
       <c r="Y44" s="6"/>
       <c r="Z44" s="6"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>212</v>
       </c>
@@ -4022,7 +4023,7 @@
       <c r="Y46" s="6"/>
       <c r="Z46" s="6"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>211</v>
       </c>
@@ -4062,7 +4063,7 @@
       <c r="Y47" s="6"/>
       <c r="Z47" s="6"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>213</v>
       </c>
@@ -4104,7 +4105,7 @@
       </c>
       <c r="Z48" s="6"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -4128,7 +4129,7 @@
       <c r="Y49" s="6"/>
       <c r="Z49" s="6"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>89</v>
       </c>
@@ -4179,7 +4180,7 @@
       <c r="Y50" s="6"/>
       <c r="Z50" s="6"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -4204,7 +4205,7 @@
       <c r="Y51" s="6"/>
       <c r="Z51" s="6"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>221</v>
       </c>
@@ -4255,7 +4256,7 @@
       </c>
       <c r="Z52" s="6"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>222</v>
       </c>
@@ -4308,7 +4309,7 @@
       </c>
       <c r="Z53" s="6"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>219</v>
       </c>
@@ -4355,7 +4356,7 @@
       </c>
       <c r="Z54" s="6"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>223</v>
       </c>
@@ -4406,7 +4407,7 @@
       </c>
       <c r="Z55" s="6"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>220</v>
       </c>
@@ -4453,7 +4454,7 @@
       </c>
       <c r="Z56" s="6"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -4477,7 +4478,7 @@
       <c r="Y57" s="6"/>
       <c r="Z57" s="6"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -4501,7 +4502,7 @@
       <c r="Y58" s="6"/>
       <c r="Z58" s="6"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>167</v>
       </c>
@@ -4535,7 +4536,7 @@
       <c r="Y59" s="6"/>
       <c r="Z59" s="6"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>167</v>
       </c>
@@ -4571,7 +4572,7 @@
       <c r="Y60" s="6"/>
       <c r="Z60" s="6"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>167</v>
       </c>
@@ -4621,7 +4622,7 @@
       <c r="Y61" s="6"/>
       <c r="Z61" s="6"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>167</v>
       </c>
@@ -4655,7 +4656,7 @@
       <c r="Y62" s="6"/>
       <c r="Z62" s="6"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -4679,7 +4680,7 @@
       <c r="Y63" s="6"/>
       <c r="Z63" s="6"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>166</v>
       </c>
@@ -4713,7 +4714,7 @@
       <c r="Y64" s="6"/>
       <c r="Z64" s="6"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>166</v>
       </c>
@@ -4747,7 +4748,7 @@
       <c r="Y65" s="6"/>
       <c r="Z65" s="6"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>166</v>
       </c>
@@ -4797,7 +4798,7 @@
       <c r="Y66" s="6"/>
       <c r="Z66" s="6"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>166</v>
       </c>
@@ -4831,7 +4832,7 @@
       </c>
       <c r="Z67" s="6"/>
     </row>
-    <row r="68" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -4855,7 +4856,7 @@
       <c r="Y68" s="6"/>
       <c r="Z68" s="6"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>165</v>
       </c>
@@ -4891,7 +4892,7 @@
       <c r="Y69" s="6"/>
       <c r="Z69" s="6"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>165</v>
       </c>
@@ -4925,7 +4926,7 @@
       <c r="Y70" s="6"/>
       <c r="Z70" s="6"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>165</v>
       </c>
@@ -4972,7 +4973,7 @@
       <c r="Y71" s="6"/>
       <c r="Z71" s="6"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>165</v>
       </c>
@@ -5004,7 +5005,7 @@
       <c r="Y72" s="6"/>
       <c r="Z72" s="6"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>50</v>
       </c>
@@ -5051,7 +5052,7 @@
       </c>
       <c r="Z74" s="6"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>49</v>
       </c>
@@ -5095,7 +5096,7 @@
       </c>
       <c r="Z75" s="6"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
         <v>134</v>
       </c>
@@ -5121,12 +5122,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I77" s="4"/>
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
         <v>235</v>
       </c>
@@ -5146,7 +5147,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>235</v>
       </c>
@@ -5160,7 +5161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
         <v>235</v>
       </c>
@@ -5174,7 +5175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
         <v>235</v>
       </c>
@@ -5188,7 +5189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
         <v>235</v>
       </c>
@@ -5202,7 +5203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="9" t="s">
         <v>235</v>
       </c>
@@ -5216,7 +5217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="s">
         <v>235</v>
       </c>
@@ -5230,7 +5231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="s">
         <v>235</v>
       </c>
@@ -5244,7 +5245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="s">
         <v>235</v>
       </c>
@@ -5258,7 +5259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
         <v>235</v>
       </c>
@@ -5272,7 +5273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="9" t="s">
         <v>235</v>
       </c>
@@ -5286,7 +5287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="9" t="s">
         <v>235</v>
       </c>
@@ -5300,7 +5301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="9" t="s">
         <v>235</v>
       </c>
@@ -5314,7 +5315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
         <v>235</v>
       </c>
@@ -5328,7 +5329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
         <v>235</v>
       </c>
@@ -5342,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="s">
         <v>235</v>
       </c>
@@ -5373,13 +5374,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7265625" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -5390,7 +5391,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -5401,7 +5402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -5412,7 +5413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -5420,7 +5421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>101</v>
       </c>

</xml_diff>